<commit_message>
perdhesa done katet ob 2
</commit_message>
<xml_diff>
--- a/2966-2/3-Katet/regjistri/29-Koordinatat-e-kateve-2966-2-Ferizaj-Armendi-leg.xlsx
+++ b/2966-2/3-Katet/regjistri/29-Koordinatat-e-kateve-2966-2-Ferizaj-Armendi-leg.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Ferizaj\Ferizaj\Ingjinierike\2966-1-Ferizaj-Armendi-leg\2966-1\3-Katet\regjistri\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Ferizaj\Ferizaj\Ingjinierike\2966-1-Ferizaj-Armendi-leg\2966-2\3-Katet\regjistri\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{013B0F0F-72B5-479C-9157-9AC100ACFEBC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5C8D562C-11ED-4512-90BA-43B07F3DC9BC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="870" yWindow="255" windowWidth="27930" windowHeight="15945" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -510,6 +510,63 @@
     <xf numFmtId="2" fontId="4" fillId="0" borderId="26" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="2" fontId="2" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="2" fillId="0" borderId="22" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="2" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="2" fillId="0" borderId="23" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="2" fillId="0" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="2" fontId="2" fillId="0" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="2" fontId="2" fillId="0" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="4" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -540,9 +597,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="2" fontId="4" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="2" fontId="4" fillId="0" borderId="24" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -551,60 +605,6 @@
     </xf>
     <xf numFmtId="2" fontId="4" fillId="0" borderId="26" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="2" fontId="2" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="2" fillId="0" borderId="22" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="2" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="2" fillId="0" borderId="23" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="2" fillId="0" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="2" fontId="2" fillId="0" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="2" fontId="2" fillId="0" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -876,7 +876,7 @@
               <a:latin typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
               <a:cs typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
             </a:rPr>
-            <a:t>: 00925-41</a:t>
+            <a:t>: 02966-2</a:t>
           </a:r>
         </a:p>
       </xdr:txBody>
@@ -1246,8 +1246,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:K61"/>
   <sheetViews>
-    <sheetView tabSelected="1" view="pageBreakPreview" topLeftCell="A16" zoomScale="85" zoomScaleNormal="100" zoomScaleSheetLayoutView="85" workbookViewId="0">
-      <selection activeCell="H31" sqref="H31:I41"/>
+    <sheetView tabSelected="1" view="pageBreakPreview" zoomScale="85" zoomScaleNormal="100" zoomScaleSheetLayoutView="85" workbookViewId="0">
+      <selection activeCell="D17" sqref="D17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1263,115 +1263,115 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="17"/>
-      <c r="B1" s="17"/>
-      <c r="C1" s="17"/>
-      <c r="D1" s="17"/>
-      <c r="E1" s="17"/>
-      <c r="F1" s="17"/>
-      <c r="G1" s="17"/>
-      <c r="H1" s="17"/>
-      <c r="I1" s="17"/>
-      <c r="J1" s="17"/>
-      <c r="K1" s="17"/>
+      <c r="A1" s="36"/>
+      <c r="B1" s="36"/>
+      <c r="C1" s="36"/>
+      <c r="D1" s="36"/>
+      <c r="E1" s="36"/>
+      <c r="F1" s="36"/>
+      <c r="G1" s="36"/>
+      <c r="H1" s="36"/>
+      <c r="I1" s="36"/>
+      <c r="J1" s="36"/>
+      <c r="K1" s="36"/>
     </row>
     <row r="2" spans="1:11" ht="62.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="17"/>
-      <c r="B2" s="17"/>
-      <c r="C2" s="17"/>
-      <c r="D2" s="17"/>
-      <c r="E2" s="17"/>
-      <c r="F2" s="17"/>
-      <c r="G2" s="17"/>
-      <c r="H2" s="17"/>
-      <c r="I2" s="17"/>
-      <c r="J2" s="17"/>
-      <c r="K2" s="17"/>
+      <c r="A2" s="36"/>
+      <c r="B2" s="36"/>
+      <c r="C2" s="36"/>
+      <c r="D2" s="36"/>
+      <c r="E2" s="36"/>
+      <c r="F2" s="36"/>
+      <c r="G2" s="36"/>
+      <c r="H2" s="36"/>
+      <c r="I2" s="36"/>
+      <c r="J2" s="36"/>
+      <c r="K2" s="36"/>
     </row>
     <row r="3" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="35" t="s">
+      <c r="A3" s="21" t="s">
         <v>9</v>
       </c>
-      <c r="B3" s="35"/>
-      <c r="C3" s="35"/>
-      <c r="D3" s="35"/>
-      <c r="E3" s="35"/>
-      <c r="F3" s="35"/>
-      <c r="G3" s="35"/>
-      <c r="H3" s="35"/>
-      <c r="I3" s="35"/>
-      <c r="J3" s="35"/>
-      <c r="K3" s="35"/>
+      <c r="B3" s="21"/>
+      <c r="C3" s="21"/>
+      <c r="D3" s="21"/>
+      <c r="E3" s="21"/>
+      <c r="F3" s="21"/>
+      <c r="G3" s="21"/>
+      <c r="H3" s="21"/>
+      <c r="I3" s="21"/>
+      <c r="J3" s="21"/>
+      <c r="K3" s="21"/>
     </row>
     <row r="4" spans="1:11" ht="28.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="35"/>
-      <c r="B4" s="35"/>
-      <c r="C4" s="35"/>
-      <c r="D4" s="35"/>
-      <c r="E4" s="35"/>
-      <c r="F4" s="35"/>
-      <c r="G4" s="35"/>
-      <c r="H4" s="35"/>
-      <c r="I4" s="35"/>
-      <c r="J4" s="35"/>
-      <c r="K4" s="35"/>
+      <c r="A4" s="21"/>
+      <c r="B4" s="21"/>
+      <c r="C4" s="21"/>
+      <c r="D4" s="21"/>
+      <c r="E4" s="21"/>
+      <c r="F4" s="21"/>
+      <c r="G4" s="21"/>
+      <c r="H4" s="21"/>
+      <c r="I4" s="21"/>
+      <c r="J4" s="21"/>
+      <c r="K4" s="21"/>
     </row>
     <row r="5" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A5" s="35"/>
-      <c r="B5" s="35"/>
-      <c r="C5" s="35"/>
-      <c r="D5" s="35"/>
-      <c r="E5" s="35"/>
-      <c r="F5" s="35"/>
-      <c r="G5" s="35"/>
-      <c r="H5" s="35"/>
-      <c r="I5" s="35"/>
-      <c r="J5" s="35"/>
-      <c r="K5" s="35"/>
+      <c r="A5" s="21"/>
+      <c r="B5" s="21"/>
+      <c r="C5" s="21"/>
+      <c r="D5" s="21"/>
+      <c r="E5" s="21"/>
+      <c r="F5" s="21"/>
+      <c r="G5" s="21"/>
+      <c r="H5" s="21"/>
+      <c r="I5" s="21"/>
+      <c r="J5" s="21"/>
+      <c r="K5" s="21"/>
     </row>
     <row r="6" spans="1:11" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="35"/>
-      <c r="B6" s="35"/>
-      <c r="C6" s="35"/>
-      <c r="D6" s="35"/>
-      <c r="E6" s="35"/>
-      <c r="F6" s="35"/>
-      <c r="G6" s="35"/>
-      <c r="H6" s="35"/>
-      <c r="I6" s="35"/>
-      <c r="J6" s="35"/>
-      <c r="K6" s="35"/>
+      <c r="A6" s="21"/>
+      <c r="B6" s="21"/>
+      <c r="C6" s="21"/>
+      <c r="D6" s="21"/>
+      <c r="E6" s="21"/>
+      <c r="F6" s="21"/>
+      <c r="G6" s="21"/>
+      <c r="H6" s="21"/>
+      <c r="I6" s="21"/>
+      <c r="J6" s="21"/>
+      <c r="K6" s="21"/>
     </row>
     <row r="7" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="8" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="C8" s="18"/>
-      <c r="D8" s="19"/>
-      <c r="E8" s="19"/>
-      <c r="F8" s="19"/>
-      <c r="G8" s="19"/>
-      <c r="H8" s="19"/>
-      <c r="I8" s="19"/>
-      <c r="J8" s="20"/>
+      <c r="C8" s="37"/>
+      <c r="D8" s="38"/>
+      <c r="E8" s="38"/>
+      <c r="F8" s="38"/>
+      <c r="G8" s="38"/>
+      <c r="H8" s="38"/>
+      <c r="I8" s="38"/>
+      <c r="J8" s="39"/>
     </row>
     <row r="9" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="C9" s="21"/>
-      <c r="D9" s="22"/>
-      <c r="E9" s="22"/>
-      <c r="F9" s="22"/>
-      <c r="G9" s="22"/>
-      <c r="H9" s="22"/>
-      <c r="I9" s="22"/>
-      <c r="J9" s="23"/>
+      <c r="C9" s="40"/>
+      <c r="D9" s="41"/>
+      <c r="E9" s="41"/>
+      <c r="F9" s="41"/>
+      <c r="G9" s="41"/>
+      <c r="H9" s="41"/>
+      <c r="I9" s="41"/>
+      <c r="J9" s="42"/>
     </row>
     <row r="10" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C10" s="24"/>
-      <c r="D10" s="25"/>
-      <c r="E10" s="25"/>
-      <c r="F10" s="25"/>
-      <c r="G10" s="25"/>
-      <c r="H10" s="25"/>
-      <c r="I10" s="25"/>
-      <c r="J10" s="26"/>
+      <c r="C10" s="43"/>
+      <c r="D10" s="44"/>
+      <c r="E10" s="44"/>
+      <c r="F10" s="44"/>
+      <c r="G10" s="44"/>
+      <c r="H10" s="44"/>
+      <c r="I10" s="44"/>
+      <c r="J10" s="45"/>
     </row>
     <row r="12" spans="1:11" x14ac:dyDescent="0.25">
       <c r="D12" s="4"/>
@@ -1409,13 +1409,13 @@
     </row>
     <row r="15" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B15" s="11">
-        <v>36</v>
+        <v>31</v>
       </c>
       <c r="C15" s="5">
-        <v>7510641.8290999997</v>
+        <v>7510650.7379999999</v>
       </c>
       <c r="D15" s="5">
-        <v>4693478.6179</v>
+        <v>4693484.3602</v>
       </c>
       <c r="E15" s="10">
         <v>648.24800000000005</v>
@@ -1423,25 +1423,25 @@
       <c r="F15" s="10" t="s">
         <v>18</v>
       </c>
-      <c r="G15" s="27" t="s">
+      <c r="G15" s="35" t="s">
         <v>8</v>
       </c>
-      <c r="H15" s="28" t="s">
+      <c r="H15" s="46" t="s">
         <v>8</v>
       </c>
-      <c r="I15" s="28">
-        <v>98.89</v>
+      <c r="I15" s="46">
+        <v>100.872</v>
       </c>
     </row>
     <row r="16" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B16" s="11">
-        <v>37</v>
+        <v>32</v>
       </c>
       <c r="C16" s="5">
-        <v>7510639.7030999996</v>
+        <v>7510653.3530000001</v>
       </c>
       <c r="D16" s="5">
-        <v>4693477.3641999997</v>
+        <v>4693475.4371999996</v>
       </c>
       <c r="E16" s="10">
         <v>648.24800000000005</v>
@@ -1449,19 +1449,19 @@
       <c r="F16" s="10" t="s">
         <v>18</v>
       </c>
-      <c r="G16" s="27"/>
-      <c r="H16" s="29"/>
-      <c r="I16" s="29"/>
+      <c r="G16" s="35"/>
+      <c r="H16" s="47"/>
+      <c r="I16" s="47"/>
     </row>
     <row r="17" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B17" s="11">
-        <v>38</v>
+        <v>33</v>
       </c>
       <c r="C17" s="5">
-        <v>7510639.2317000004</v>
+        <v>7510655.3514</v>
       </c>
       <c r="D17" s="5">
-        <v>4693465.7909000004</v>
+        <v>4693476.6594000002</v>
       </c>
       <c r="E17" s="10">
         <v>648.24800000000005</v>
@@ -1469,19 +1469,19 @@
       <c r="F17" s="10" t="s">
         <v>18</v>
       </c>
-      <c r="G17" s="27"/>
-      <c r="H17" s="29"/>
-      <c r="I17" s="29"/>
+      <c r="G17" s="35"/>
+      <c r="H17" s="47"/>
+      <c r="I17" s="47"/>
     </row>
     <row r="18" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B18" s="11">
-        <v>39</v>
+        <v>34</v>
       </c>
       <c r="C18" s="5">
-        <v>7510638.0011</v>
+        <v>7510648.5892000003</v>
       </c>
       <c r="D18" s="5">
-        <v>4693465.0647999998</v>
+        <v>4693483.0460999999</v>
       </c>
       <c r="E18" s="10">
         <v>648.24800000000005</v>
@@ -1489,19 +1489,19 @@
       <c r="F18" s="10" t="s">
         <v>18</v>
       </c>
-      <c r="G18" s="27"/>
-      <c r="H18" s="29"/>
-      <c r="I18" s="29"/>
+      <c r="G18" s="35"/>
+      <c r="H18" s="47"/>
+      <c r="I18" s="47"/>
     </row>
     <row r="19" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B19" s="11">
-        <v>40</v>
+        <v>35</v>
       </c>
       <c r="C19" s="5">
-        <v>7510632.9046</v>
+        <v>7510641.7006000001</v>
       </c>
       <c r="D19" s="5">
-        <v>4693473.3550000004</v>
+        <v>4693478.8332000002</v>
       </c>
       <c r="E19" s="10">
         <v>648.24800000000005</v>
@@ -1509,19 +1509,19 @@
       <c r="F19" s="10" t="s">
         <v>18</v>
       </c>
-      <c r="G19" s="27"/>
-      <c r="H19" s="29"/>
-      <c r="I19" s="29"/>
+      <c r="G19" s="35"/>
+      <c r="H19" s="47"/>
+      <c r="I19" s="47"/>
     </row>
     <row r="20" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B20" s="11">
-        <v>97</v>
+        <v>103</v>
       </c>
       <c r="C20" s="5">
-        <v>7510639.2709999997</v>
+        <v>7510653.6935999999</v>
       </c>
       <c r="D20" s="5">
-        <v>4693465.727</v>
+        <v>4693474.8667000001</v>
       </c>
       <c r="E20" s="10">
         <v>648.24800000000005</v>
@@ -1529,19 +1529,19 @@
       <c r="F20" s="10" t="s">
         <v>18</v>
       </c>
-      <c r="G20" s="27"/>
-      <c r="H20" s="29"/>
-      <c r="I20" s="29"/>
+      <c r="G20" s="35"/>
+      <c r="H20" s="47"/>
+      <c r="I20" s="47"/>
     </row>
     <row r="21" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B21" s="11">
-        <v>98</v>
+        <v>104</v>
       </c>
       <c r="C21" s="5">
-        <v>7510641.0773</v>
+        <v>7510649.7476000004</v>
       </c>
       <c r="D21" s="5">
-        <v>4693466.7927000001</v>
+        <v>4693472.4534999998</v>
       </c>
       <c r="E21" s="10">
         <v>648.24800000000005</v>
@@ -1549,19 +1549,19 @@
       <c r="F21" s="10" t="s">
         <v>18</v>
       </c>
-      <c r="G21" s="27"/>
-      <c r="H21" s="29"/>
-      <c r="I21" s="29"/>
+      <c r="G21" s="35"/>
+      <c r="H21" s="47"/>
+      <c r="I21" s="47"/>
     </row>
     <row r="22" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B22" s="11">
-        <v>99</v>
+        <v>105</v>
       </c>
       <c r="C22" s="5">
-        <v>7510641.0379999997</v>
+        <v>7510649.8039999995</v>
       </c>
       <c r="D22" s="5">
-        <v>4693466.8565999996</v>
+        <v>4693472.3590000002</v>
       </c>
       <c r="E22" s="10">
         <v>648.24800000000005</v>
@@ -1569,19 +1569,19 @@
       <c r="F22" s="10" t="s">
         <v>18</v>
       </c>
-      <c r="G22" s="27"/>
-      <c r="H22" s="29"/>
-      <c r="I22" s="29"/>
+      <c r="G22" s="35"/>
+      <c r="H22" s="47"/>
+      <c r="I22" s="47"/>
     </row>
     <row r="23" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B23" s="11">
-        <v>100</v>
+        <v>106</v>
       </c>
       <c r="C23" s="5">
-        <v>7510645.0045999996</v>
+        <v>7510648.0743000004</v>
       </c>
       <c r="D23" s="5">
-        <v>4693469.1969999997</v>
+        <v>4693471.3010999998</v>
       </c>
       <c r="E23" s="10">
         <v>648.24800000000005</v>
@@ -1589,19 +1589,19 @@
       <c r="F23" s="10" t="s">
         <v>18</v>
       </c>
-      <c r="G23" s="27"/>
-      <c r="H23" s="29"/>
-      <c r="I23" s="29"/>
+      <c r="G23" s="35"/>
+      <c r="H23" s="47"/>
+      <c r="I23" s="47"/>
     </row>
     <row r="24" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B24" s="11">
-        <v>101</v>
+        <v>107</v>
       </c>
       <c r="C24" s="5">
-        <v>7510644.6449999996</v>
+        <v>7510648.0179000003</v>
       </c>
       <c r="D24" s="5">
-        <v>4693469.7819999997</v>
+        <v>4693471.3956000004</v>
       </c>
       <c r="E24" s="10">
         <v>648.24800000000005</v>
@@ -1609,19 +1609,19 @@
       <c r="F24" s="10" t="s">
         <v>18</v>
       </c>
-      <c r="G24" s="27"/>
-      <c r="H24" s="30"/>
-      <c r="I24" s="30"/>
+      <c r="G24" s="35"/>
+      <c r="H24" s="48"/>
+      <c r="I24" s="48"/>
     </row>
     <row r="25" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B25" s="11">
-        <v>102</v>
+        <v>108</v>
       </c>
       <c r="C25" s="5">
-        <v>7510646.4632999999</v>
+        <v>7510646.6425000001</v>
       </c>
       <c r="D25" s="5">
-        <v>4693470.8547999999</v>
+        <v>4693470.5544999996</v>
       </c>
       <c r="E25" s="10">
         <v>648.24800000000005</v>
@@ -1629,57 +1629,57 @@
       <c r="F25" s="10" t="s">
         <v>18</v>
       </c>
-      <c r="G25" s="27"/>
+      <c r="G25" s="35"/>
       <c r="H25" s="16" t="s">
         <v>14</v>
       </c>
       <c r="I25" s="16">
-        <v>15.148</v>
+        <v>15.7</v>
       </c>
     </row>
     <row r="26" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B26" s="11">
-        <v>19</v>
+        <v>21</v>
       </c>
       <c r="C26" s="5">
-        <v>7510638.7419999996</v>
+        <v>7510640.6648000004</v>
       </c>
       <c r="D26" s="5">
-        <v>4693478.9939999999</v>
+        <v>4693480.5681999996</v>
       </c>
       <c r="E26" s="10">
-        <v>648.21199999999999</v>
+        <v>648.24800000000005</v>
       </c>
       <c r="F26" s="10" t="s">
         <v>19</v>
       </c>
-      <c r="G26" s="27"/>
+      <c r="G26" s="35"/>
       <c r="H26" s="16"/>
       <c r="I26" s="16"/>
     </row>
     <row r="27" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B27" s="11">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="C27" s="5">
-        <v>7510631.8894999996</v>
+        <v>7510647.6119999997</v>
       </c>
       <c r="D27" s="5">
-        <v>4693475.0062999995</v>
+        <v>4693484.6440000003</v>
       </c>
       <c r="E27" s="10">
-        <v>648.24800000000005</v>
+        <v>648.25300000000004</v>
       </c>
       <c r="F27" s="10" t="s">
         <v>19</v>
       </c>
-      <c r="G27" s="27"/>
+      <c r="G27" s="35"/>
       <c r="H27" s="14" t="s">
         <v>13</v>
       </c>
       <c r="I27" s="14">
         <f>SUM(I15:I25)</f>
-        <v>114.038</v>
+        <v>116.572</v>
       </c>
     </row>
     <row r="28" spans="2:9" x14ac:dyDescent="0.25">
@@ -1740,13 +1740,13 @@
       <c r="F31" s="10" t="s">
         <v>17</v>
       </c>
-      <c r="G31" s="27" t="s">
+      <c r="G31" s="35" t="s">
         <v>16</v>
       </c>
-      <c r="H31" s="27" t="s">
+      <c r="H31" s="35" t="s">
         <v>16</v>
       </c>
-      <c r="I31" s="27">
+      <c r="I31" s="35">
         <v>79.843000000000004</v>
       </c>
     </row>
@@ -1766,9 +1766,9 @@
       <c r="F32" s="10" t="s">
         <v>17</v>
       </c>
-      <c r="G32" s="27"/>
-      <c r="H32" s="27"/>
-      <c r="I32" s="27"/>
+      <c r="G32" s="35"/>
+      <c r="H32" s="35"/>
+      <c r="I32" s="35"/>
     </row>
     <row r="33" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B33" s="11">
@@ -1786,9 +1786,9 @@
       <c r="F33" s="10" t="s">
         <v>17</v>
       </c>
-      <c r="G33" s="27"/>
-      <c r="H33" s="27"/>
-      <c r="I33" s="27"/>
+      <c r="G33" s="35"/>
+      <c r="H33" s="35"/>
+      <c r="I33" s="35"/>
     </row>
     <row r="34" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B34" s="11">
@@ -1806,9 +1806,9 @@
       <c r="F34" s="10" t="s">
         <v>17</v>
       </c>
-      <c r="G34" s="27"/>
-      <c r="H34" s="27"/>
-      <c r="I34" s="27"/>
+      <c r="G34" s="35"/>
+      <c r="H34" s="35"/>
+      <c r="I34" s="35"/>
     </row>
     <row r="35" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B35" s="11">
@@ -1826,9 +1826,9 @@
       <c r="F35" s="10" t="s">
         <v>17</v>
       </c>
-      <c r="G35" s="27"/>
-      <c r="H35" s="27"/>
-      <c r="I35" s="27"/>
+      <c r="G35" s="35"/>
+      <c r="H35" s="35"/>
+      <c r="I35" s="35"/>
     </row>
     <row r="36" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B36" s="11">
@@ -1846,9 +1846,9 @@
       <c r="F36" s="10" t="s">
         <v>17</v>
       </c>
-      <c r="G36" s="27"/>
-      <c r="H36" s="27"/>
-      <c r="I36" s="27"/>
+      <c r="G36" s="35"/>
+      <c r="H36" s="35"/>
+      <c r="I36" s="35"/>
     </row>
     <row r="37" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B37" s="11">
@@ -1866,9 +1866,9 @@
       <c r="F37" s="10" t="s">
         <v>17</v>
       </c>
-      <c r="G37" s="27"/>
-      <c r="H37" s="27"/>
-      <c r="I37" s="27"/>
+      <c r="G37" s="35"/>
+      <c r="H37" s="35"/>
+      <c r="I37" s="35"/>
     </row>
     <row r="38" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B38" s="11">
@@ -1886,9 +1886,9 @@
       <c r="F38" s="10" t="s">
         <v>17</v>
       </c>
-      <c r="G38" s="27"/>
-      <c r="H38" s="27"/>
-      <c r="I38" s="27"/>
+      <c r="G38" s="35"/>
+      <c r="H38" s="35"/>
+      <c r="I38" s="35"/>
     </row>
     <row r="39" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B39" s="11">
@@ -1906,7 +1906,7 @@
       <c r="F39" s="10" t="s">
         <v>17</v>
       </c>
-      <c r="G39" s="27"/>
+      <c r="G39" s="35"/>
       <c r="H39" s="10" t="s">
         <v>14</v>
       </c>
@@ -1930,7 +1930,7 @@
       <c r="F40" s="10" t="s">
         <v>22</v>
       </c>
-      <c r="G40" s="27"/>
+      <c r="G40" s="35"/>
       <c r="H40" s="10"/>
       <c r="I40" s="10"/>
     </row>
@@ -1950,7 +1950,7 @@
       <c r="F41" s="10" t="s">
         <v>22</v>
       </c>
-      <c r="G41" s="27"/>
+      <c r="G41" s="35"/>
       <c r="H41" s="14" t="s">
         <v>13</v>
       </c>
@@ -2017,13 +2017,13 @@
       <c r="F45" s="10" t="s">
         <v>20</v>
       </c>
-      <c r="G45" s="27" t="s">
+      <c r="G45" s="35" t="s">
         <v>21</v>
       </c>
-      <c r="H45" s="27" t="s">
+      <c r="H45" s="35" t="s">
         <v>21</v>
       </c>
-      <c r="I45" s="27">
+      <c r="I45" s="35">
         <v>49.24</v>
       </c>
     </row>
@@ -2043,9 +2043,9 @@
       <c r="F46" s="10" t="s">
         <v>20</v>
       </c>
-      <c r="G46" s="27"/>
-      <c r="H46" s="27"/>
-      <c r="I46" s="27"/>
+      <c r="G46" s="35"/>
+      <c r="H46" s="35"/>
+      <c r="I46" s="35"/>
     </row>
     <row r="47" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B47" s="11">
@@ -2063,9 +2063,9 @@
       <c r="F47" s="10" t="s">
         <v>20</v>
       </c>
-      <c r="G47" s="27"/>
-      <c r="H47" s="27"/>
-      <c r="I47" s="27"/>
+      <c r="G47" s="35"/>
+      <c r="H47" s="35"/>
+      <c r="I47" s="35"/>
     </row>
     <row r="48" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B48" s="11">
@@ -2083,9 +2083,9 @@
       <c r="F48" s="10" t="s">
         <v>20</v>
       </c>
-      <c r="G48" s="27"/>
-      <c r="H48" s="27"/>
-      <c r="I48" s="27"/>
+      <c r="G48" s="35"/>
+      <c r="H48" s="35"/>
+      <c r="I48" s="35"/>
     </row>
     <row r="49" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B49" s="11">
@@ -2103,9 +2103,9 @@
       <c r="F49" s="10" t="s">
         <v>20</v>
       </c>
-      <c r="G49" s="27"/>
-      <c r="H49" s="27"/>
-      <c r="I49" s="27"/>
+      <c r="G49" s="35"/>
+      <c r="H49" s="35"/>
+      <c r="I49" s="35"/>
     </row>
     <row r="50" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B50" s="11">
@@ -2123,9 +2123,9 @@
       <c r="F50" s="10" t="s">
         <v>20</v>
       </c>
-      <c r="G50" s="27"/>
-      <c r="H50" s="27"/>
-      <c r="I50" s="27"/>
+      <c r="G50" s="35"/>
+      <c r="H50" s="35"/>
+      <c r="I50" s="35"/>
     </row>
     <row r="51" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B51" s="11">
@@ -2143,7 +2143,7 @@
       <c r="F51" s="10" t="s">
         <v>20</v>
       </c>
-      <c r="G51" s="27"/>
+      <c r="G51" s="35"/>
       <c r="H51" s="15"/>
       <c r="I51" s="15"/>
     </row>
@@ -2163,7 +2163,7 @@
       <c r="F52" s="10" t="s">
         <v>20</v>
       </c>
-      <c r="G52" s="27"/>
+      <c r="G52" s="35"/>
       <c r="H52" s="14" t="s">
         <v>13</v>
       </c>
@@ -2206,34 +2206,34 @@
       <c r="B57" s="3"/>
       <c r="C57" s="3"/>
       <c r="D57" s="3"/>
-      <c r="E57" s="40" t="s">
+      <c r="E57" s="26" t="s">
         <v>15</v>
       </c>
-      <c r="F57" s="41"/>
-      <c r="G57" s="42"/>
-      <c r="H57" s="36" t="s">
+      <c r="F57" s="27"/>
+      <c r="G57" s="28"/>
+      <c r="H57" s="22" t="s">
         <v>4</v>
       </c>
-      <c r="I57" s="37"/>
-      <c r="J57" s="31"/>
-      <c r="K57" s="32"/>
+      <c r="I57" s="23"/>
+      <c r="J57" s="17"/>
+      <c r="K57" s="18"/>
     </row>
     <row r="58" spans="1:11" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A58" s="43" t="s">
+      <c r="A58" s="29" t="s">
         <v>3</v>
       </c>
-      <c r="B58" s="44"/>
-      <c r="C58" s="44"/>
-      <c r="D58" s="45"/>
-      <c r="E58" s="46">
+      <c r="B58" s="30"/>
+      <c r="C58" s="30"/>
+      <c r="D58" s="31"/>
+      <c r="E58" s="32">
         <v>140</v>
       </c>
-      <c r="F58" s="47"/>
-      <c r="G58" s="48"/>
-      <c r="H58" s="38"/>
-      <c r="I58" s="39"/>
-      <c r="J58" s="33"/>
-      <c r="K58" s="34"/>
+      <c r="F58" s="33"/>
+      <c r="G58" s="34"/>
+      <c r="H58" s="24"/>
+      <c r="I58" s="25"/>
+      <c r="J58" s="19"/>
+      <c r="K58" s="20"/>
     </row>
     <row r="59" spans="1:11" ht="18.75" x14ac:dyDescent="0.3">
       <c r="K59" s="1"/>
@@ -2246,6 +2246,11 @@
     </row>
   </sheetData>
   <mergeCells count="17">
+    <mergeCell ref="A1:K2"/>
+    <mergeCell ref="C8:J10"/>
+    <mergeCell ref="G15:G27"/>
+    <mergeCell ref="H15:H24"/>
+    <mergeCell ref="I15:I24"/>
     <mergeCell ref="J57:K58"/>
     <mergeCell ref="A3:K6"/>
     <mergeCell ref="H57:I58"/>
@@ -2258,11 +2263,6 @@
     <mergeCell ref="G45:G52"/>
     <mergeCell ref="H45:H50"/>
     <mergeCell ref="I45:I50"/>
-    <mergeCell ref="A1:K2"/>
-    <mergeCell ref="C8:J10"/>
-    <mergeCell ref="G15:G27"/>
-    <mergeCell ref="H15:H24"/>
-    <mergeCell ref="I15:I24"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" scale="58" orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId1"/>

</xml_diff>

<commit_message>
kati 1 done ob 2
</commit_message>
<xml_diff>
--- a/2966-2/3-Katet/regjistri/29-Koordinatat-e-kateve-2966-2-Ferizaj-Armendi-leg.xlsx
+++ b/2966-2/3-Katet/regjistri/29-Koordinatat-e-kateve-2966-2-Ferizaj-Armendi-leg.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Ferizaj\Ferizaj\Ingjinierike\2966-1-Ferizaj-Armendi-leg\2966-2\3-Katet\regjistri\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CC51C645-5032-4AD5-9417-B9FD90E8C13D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6C22FBF0-CEEA-4DA7-AE54-E6BDDD2B9504}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="870" yWindow="255" windowWidth="27930" windowHeight="15945" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1246,8 +1246,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:K61"/>
   <sheetViews>
-    <sheetView tabSelected="1" view="pageBreakPreview" topLeftCell="A22" zoomScale="85" zoomScaleNormal="100" zoomScaleSheetLayoutView="85" workbookViewId="0">
-      <selection activeCell="J51" sqref="J51"/>
+    <sheetView tabSelected="1" view="pageBreakPreview" topLeftCell="A19" zoomScale="85" zoomScaleNormal="100" zoomScaleSheetLayoutView="85" workbookViewId="0">
+      <selection activeCell="F36" sqref="B30:I41"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1726,13 +1726,13 @@
     </row>
     <row r="31" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B31" s="11">
-        <v>53</v>
+        <v>50</v>
       </c>
       <c r="C31" s="5">
-        <v>7510640.0105999997</v>
+        <v>7510648.7396</v>
       </c>
       <c r="D31" s="5">
-        <v>4693477.5455</v>
+        <v>4693483.1380000003</v>
       </c>
       <c r="E31" s="10">
         <v>651.38900000000001</v>
@@ -1747,18 +1747,18 @@
         <v>16</v>
       </c>
       <c r="I31" s="35">
-        <v>79.843000000000004</v>
+        <v>79.843999999999994</v>
       </c>
     </row>
     <row r="32" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B32" s="11">
-        <v>54</v>
+        <v>51</v>
       </c>
       <c r="C32" s="5">
-        <v>7510632.9046</v>
+        <v>7510648.5892000003</v>
       </c>
       <c r="D32" s="5">
-        <v>4693473.3550000004</v>
+        <v>4693483.0460999999</v>
       </c>
       <c r="E32" s="10">
         <v>651.38900000000001</v>
@@ -1772,13 +1772,13 @@
     </row>
     <row r="33" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B33" s="11">
-        <v>65</v>
+        <v>52</v>
       </c>
       <c r="C33" s="5">
-        <v>7510639.7030999996</v>
+        <v>7510641.7006000001</v>
       </c>
       <c r="D33" s="5">
-        <v>4693477.3641999997</v>
+        <v>4693478.8332000002</v>
       </c>
       <c r="E33" s="10">
         <v>651.38900000000001</v>
@@ -1792,13 +1792,13 @@
     </row>
     <row r="34" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B34" s="11">
-        <v>67</v>
+        <v>60</v>
       </c>
       <c r="C34" s="5">
-        <v>7510644.9709999999</v>
+        <v>7510653.6935999999</v>
       </c>
       <c r="D34" s="5">
-        <v>4693469.2079999996</v>
+        <v>4693474.8667000001</v>
       </c>
       <c r="E34" s="10">
         <v>651.38900000000001</v>
@@ -1812,13 +1812,13 @@
     </row>
     <row r="35" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B35" s="11">
-        <v>68</v>
+        <v>61</v>
       </c>
       <c r="C35" s="5">
-        <v>7510641.0379999997</v>
+        <v>7510649.8039999995</v>
       </c>
       <c r="D35" s="5">
-        <v>4693466.8565999996</v>
+        <v>4693472.3590000002</v>
       </c>
       <c r="E35" s="10">
         <v>651.38900000000001</v>
@@ -1832,13 +1832,13 @@
     </row>
     <row r="36" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B36" s="11">
-        <v>69</v>
+        <v>62</v>
       </c>
       <c r="C36" s="5">
-        <v>7510641.0789999999</v>
+        <v>7510648.0659999996</v>
       </c>
       <c r="D36" s="5">
-        <v>4693466.79</v>
+        <v>4693471.3150000004</v>
       </c>
       <c r="E36" s="10">
         <v>651.38900000000001</v>
@@ -1852,13 +1852,13 @@
     </row>
     <row r="37" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B37" s="11">
-        <v>70</v>
+        <v>63</v>
       </c>
       <c r="C37" s="5">
-        <v>7510639.2709999997</v>
+        <v>7510648.0179000003</v>
       </c>
       <c r="D37" s="5">
-        <v>4693465.727</v>
+        <v>4693471.3956000004</v>
       </c>
       <c r="E37" s="10">
         <v>651.38900000000001</v>
@@ -1872,13 +1872,13 @@
     </row>
     <row r="38" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B38" s="11">
-        <v>71</v>
+        <v>64</v>
       </c>
       <c r="C38" s="5">
-        <v>7510639.2317000004</v>
+        <v>7510646.6425000001</v>
       </c>
       <c r="D38" s="5">
-        <v>4693465.7909000004</v>
+        <v>4693470.5544999996</v>
       </c>
       <c r="E38" s="10">
         <v>651.38900000000001</v>
@@ -1892,13 +1892,13 @@
     </row>
     <row r="39" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B39" s="11">
-        <v>72</v>
+        <v>75</v>
       </c>
       <c r="C39" s="5">
-        <v>7510638.0011</v>
+        <v>7510649.7476000004</v>
       </c>
       <c r="D39" s="5">
-        <v>4693465.0647999998</v>
+        <v>4693472.4534999998</v>
       </c>
       <c r="E39" s="10">
         <v>651.38900000000001</v>
@@ -1911,18 +1911,18 @@
         <v>14</v>
       </c>
       <c r="I39" s="10">
-        <v>7.6779999999999999</v>
+        <v>8.3149999999999995</v>
       </c>
     </row>
     <row r="40" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B40" s="11">
-        <v>41</v>
+        <v>43</v>
       </c>
       <c r="C40" s="5">
-        <v>7510632.3836000003</v>
+        <v>7510641.1344999997</v>
       </c>
       <c r="D40" s="5">
-        <v>4693474.2024999997</v>
+        <v>4693479.7813999997</v>
       </c>
       <c r="E40" s="10">
         <v>651.38900000000001</v>
@@ -1936,13 +1936,13 @@
     </row>
     <row r="41" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B41" s="11">
-        <v>42</v>
+        <v>44</v>
       </c>
       <c r="C41" s="5">
-        <v>7510639.2210999997</v>
+        <v>7510648.0900999997</v>
       </c>
       <c r="D41" s="5">
-        <v>4693478.1814999999</v>
+        <v>4693483.8622000003</v>
       </c>
       <c r="E41" s="10">
         <v>651.38900000000001</v>
@@ -1956,7 +1956,7 @@
       </c>
       <c r="I41" s="14">
         <f>SUM(I31:I39)</f>
-        <v>87.521000000000001</v>
+        <v>88.158999999999992</v>
       </c>
     </row>
     <row r="42" spans="2:9" x14ac:dyDescent="0.25">

</xml_diff>